<commit_message>
Addet Unit testing for available commands
</commit_message>
<xml_diff>
--- a/CommandSetDescribeD0.6ver2.xlsx
+++ b/CommandSetDescribeD0.6ver2.xlsx
@@ -18,8 +18,8 @@
   </sheets>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Chathuranga Dissanayaka - Personal View" guid="{808BDE38-2E40-4450-8137-228A8C80B0DE}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1616" windowHeight="886" activeSheetId="1"/>
     <customWorkbookView name="Kanishka Wijayasekara - Personal View" guid="{71292C98-6F74-4667-9CC4-FC968CFB3932}" mergeInterval="0" personalView="1" maximized="1" xWindow="1358" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
-    <customWorkbookView name="Chathuranga Dissanayaka - Personal View" guid="{808BDE38-2E40-4450-8137-228A8C80B0DE}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1616" windowHeight="886" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2646,9 +2646,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2699,6 +2696,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2982,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="C425" sqref="C425"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="D413" sqref="D413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2995,11 +2995,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -3014,18 +3014,18 @@
       <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -3094,11 +3094,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -3178,18 +3178,18 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -3258,11 +3258,11 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -3342,18 +3342,18 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="27"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -3422,11 +3422,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="30"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="29"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -3506,18 +3506,18 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="27"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="26"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
@@ -3586,11 +3586,11 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="30"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="29"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -3670,18 +3670,18 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="s">
+      <c r="A69" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B69" s="26"/>
-      <c r="C69" s="27"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="26"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -3750,11 +3750,11 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B76" s="29"/>
-      <c r="C76" s="30"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="29"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -3834,18 +3834,18 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="23" t="s">
+      <c r="A84" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="23"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B85" s="26"/>
-      <c r="C85" s="27"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="26"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
@@ -3914,11 +3914,11 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B92" s="29"/>
-      <c r="C92" s="30"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="29"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
@@ -4009,18 +4009,18 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="23" t="s">
+      <c r="A101" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="23"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="25" t="s">
+      <c r="A102" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="26"/>
-      <c r="C102" s="27"/>
+      <c r="B102" s="25"/>
+      <c r="C102" s="26"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
@@ -4089,11 +4089,11 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="28" t="s">
+      <c r="A109" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B109" s="29"/>
-      <c r="C109" s="30"/>
+      <c r="B109" s="28"/>
+      <c r="C109" s="29"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
@@ -4184,18 +4184,18 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="23" t="s">
+      <c r="A118" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B118" s="24"/>
-      <c r="C118" s="24"/>
+      <c r="B118" s="23"/>
+      <c r="C118" s="23"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="25" t="s">
+      <c r="A119" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B119" s="26"/>
-      <c r="C119" s="27"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="26"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
@@ -4264,11 +4264,11 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="28" t="s">
+      <c r="A126" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B126" s="29"/>
-      <c r="C126" s="30"/>
+      <c r="B126" s="28"/>
+      <c r="C126" s="29"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
@@ -4366,18 +4366,18 @@
       <c r="C137" s="21"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="23" t="s">
+      <c r="A138" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B138" s="24"/>
-      <c r="C138" s="24"/>
+      <c r="B138" s="23"/>
+      <c r="C138" s="23"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="25" t="s">
+      <c r="A139" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B139" s="26"/>
-      <c r="C139" s="27"/>
+      <c r="B139" s="25"/>
+      <c r="C139" s="26"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
@@ -4446,11 +4446,11 @@
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="28" t="s">
+      <c r="A146" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B146" s="29"/>
-      <c r="C146" s="30"/>
+      <c r="B146" s="28"/>
+      <c r="C146" s="29"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
@@ -4541,11 +4541,11 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="37" t="s">
+      <c r="A155" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="B155" s="38"/>
-      <c r="C155" s="39"/>
+      <c r="B155" s="37"/>
+      <c r="C155" s="38"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
@@ -4726,25 +4726,25 @@
       <c r="C173" s="11"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="31" t="s">
+      <c r="A174" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B174" s="32"/>
-      <c r="C174" s="33"/>
+      <c r="B174" s="31"/>
+      <c r="C174" s="32"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="34" t="s">
+      <c r="A175" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B175" s="35"/>
-      <c r="C175" s="36"/>
+      <c r="B175" s="34"/>
+      <c r="C175" s="35"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="25" t="s">
+      <c r="A176" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B176" s="26"/>
-      <c r="C176" s="27"/>
+      <c r="B176" s="25"/>
+      <c r="C176" s="26"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
@@ -4813,11 +4813,11 @@
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="28" t="s">
+      <c r="A183" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B183" s="29"/>
-      <c r="C183" s="30"/>
+      <c r="B183" s="28"/>
+      <c r="C183" s="29"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
@@ -4897,18 +4897,18 @@
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="23" t="s">
+      <c r="A191" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B191" s="24"/>
-      <c r="C191" s="24"/>
+      <c r="B191" s="23"/>
+      <c r="C191" s="23"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="25" t="s">
+      <c r="A192" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B192" s="26"/>
-      <c r="C192" s="27"/>
+      <c r="B192" s="25"/>
+      <c r="C192" s="26"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
@@ -4977,11 +4977,11 @@
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="28" t="s">
+      <c r="A199" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B199" s="29"/>
-      <c r="C199" s="30"/>
+      <c r="B199" s="28"/>
+      <c r="C199" s="29"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
@@ -5061,18 +5061,18 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="23" t="s">
+      <c r="A207" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B207" s="24"/>
-      <c r="C207" s="24"/>
+      <c r="B207" s="23"/>
+      <c r="C207" s="23"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="25" t="s">
+      <c r="A208" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B208" s="26"/>
-      <c r="C208" s="27"/>
+      <c r="B208" s="25"/>
+      <c r="C208" s="26"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
@@ -5141,11 +5141,11 @@
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="28" t="s">
+      <c r="A215" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B215" s="29"/>
-      <c r="C215" s="30"/>
+      <c r="B215" s="28"/>
+      <c r="C215" s="29"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
@@ -5225,18 +5225,18 @@
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" s="23" t="s">
+      <c r="A223" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B223" s="24"/>
-      <c r="C223" s="24"/>
+      <c r="B223" s="23"/>
+      <c r="C223" s="23"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="25" t="s">
+      <c r="A224" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B224" s="26"/>
-      <c r="C224" s="27"/>
+      <c r="B224" s="25"/>
+      <c r="C224" s="26"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
@@ -5316,11 +5316,11 @@
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="28" t="s">
+      <c r="A232" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B232" s="29"/>
-      <c r="C232" s="30"/>
+      <c r="B232" s="28"/>
+      <c r="C232" s="29"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
@@ -5407,18 +5407,18 @@
       <c r="C242" s="21"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="23" t="s">
+      <c r="A243" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B243" s="24"/>
-      <c r="C243" s="24"/>
+      <c r="B243" s="23"/>
+      <c r="C243" s="23"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="25" t="s">
+      <c r="A244" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B244" s="26"/>
-      <c r="C244" s="27"/>
+      <c r="B244" s="25"/>
+      <c r="C244" s="26"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
@@ -5498,11 +5498,11 @@
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="28" t="s">
+      <c r="A252" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B252" s="29"/>
-      <c r="C252" s="30"/>
+      <c r="B252" s="28"/>
+      <c r="C252" s="29"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
@@ -5582,18 +5582,18 @@
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="23" t="s">
+      <c r="A260" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B260" s="24"/>
-      <c r="C260" s="24"/>
+      <c r="B260" s="23"/>
+      <c r="C260" s="23"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="25" t="s">
+      <c r="A261" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B261" s="26"/>
-      <c r="C261" s="27"/>
+      <c r="B261" s="25"/>
+      <c r="C261" s="26"/>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
@@ -5673,11 +5673,11 @@
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="28" t="s">
+      <c r="A269" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B269" s="29"/>
-      <c r="C269" s="30"/>
+      <c r="B269" s="28"/>
+      <c r="C269" s="29"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
@@ -5764,18 +5764,18 @@
       <c r="C279" s="21"/>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" s="23" t="s">
+      <c r="A280" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B280" s="24"/>
-      <c r="C280" s="24"/>
+      <c r="B280" s="23"/>
+      <c r="C280" s="23"/>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" s="25" t="s">
+      <c r="A281" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B281" s="26"/>
-      <c r="C281" s="27"/>
+      <c r="B281" s="25"/>
+      <c r="C281" s="26"/>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
@@ -5844,11 +5844,11 @@
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="28" t="s">
+      <c r="A288" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B288" s="29"/>
-      <c r="C288" s="30"/>
+      <c r="B288" s="28"/>
+      <c r="C288" s="29"/>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
@@ -5928,18 +5928,18 @@
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A296" s="23" t="s">
+      <c r="A296" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B296" s="24"/>
-      <c r="C296" s="24"/>
+      <c r="B296" s="23"/>
+      <c r="C296" s="23"/>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297" s="25" t="s">
+      <c r="A297" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B297" s="26"/>
-      <c r="C297" s="27"/>
+      <c r="B297" s="25"/>
+      <c r="C297" s="26"/>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
@@ -6008,11 +6008,11 @@
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304" s="28" t="s">
+      <c r="A304" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B304" s="29"/>
-      <c r="C304" s="30"/>
+      <c r="B304" s="28"/>
+      <c r="C304" s="29"/>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
@@ -6092,18 +6092,18 @@
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" s="23" t="s">
+      <c r="A312" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B312" s="24"/>
-      <c r="C312" s="24"/>
+      <c r="B312" s="23"/>
+      <c r="C312" s="23"/>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A313" s="25" t="s">
+      <c r="A313" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B313" s="26"/>
-      <c r="C313" s="27"/>
+      <c r="B313" s="25"/>
+      <c r="C313" s="26"/>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
@@ -6183,11 +6183,11 @@
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" s="28" t="s">
+      <c r="A321" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B321" s="29"/>
-      <c r="C321" s="30"/>
+      <c r="B321" s="28"/>
+      <c r="C321" s="29"/>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
@@ -6279,18 +6279,18 @@
       <c r="C331" s="21"/>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A332" s="23" t="s">
+      <c r="A332" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B332" s="24"/>
-      <c r="C332" s="24"/>
+      <c r="B332" s="23"/>
+      <c r="C332" s="23"/>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A333" s="25" t="s">
+      <c r="A333" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B333" s="26"/>
-      <c r="C333" s="27"/>
+      <c r="B333" s="25"/>
+      <c r="C333" s="26"/>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
@@ -6359,11 +6359,11 @@
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A340" s="28" t="s">
+      <c r="A340" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B340" s="29"/>
-      <c r="C340" s="30"/>
+      <c r="B340" s="28"/>
+      <c r="C340" s="29"/>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
@@ -6454,18 +6454,18 @@
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A349" s="23" t="s">
+      <c r="A349" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B349" s="24"/>
-      <c r="C349" s="24"/>
+      <c r="B349" s="23"/>
+      <c r="C349" s="23"/>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A350" s="25" t="s">
+      <c r="A350" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B350" s="26"/>
-      <c r="C350" s="27"/>
+      <c r="B350" s="25"/>
+      <c r="C350" s="26"/>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
@@ -6556,11 +6556,11 @@
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A359" s="28" t="s">
+      <c r="A359" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B359" s="29"/>
-      <c r="C359" s="30"/>
+      <c r="B359" s="28"/>
+      <c r="C359" s="29"/>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
@@ -6657,18 +6657,18 @@
       <c r="C370" s="21"/>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A371" s="23" t="s">
+      <c r="A371" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B371" s="24"/>
-      <c r="C371" s="24"/>
+      <c r="B371" s="23"/>
+      <c r="C371" s="23"/>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A372" s="25" t="s">
+      <c r="A372" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B372" s="26"/>
-      <c r="C372" s="27"/>
+      <c r="B372" s="25"/>
+      <c r="C372" s="26"/>
     </row>
     <row r="373" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
@@ -6737,11 +6737,11 @@
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A379" s="28" t="s">
+      <c r="A379" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B379" s="29"/>
-      <c r="C379" s="30"/>
+      <c r="B379" s="28"/>
+      <c r="C379" s="29"/>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
@@ -6828,18 +6828,18 @@
       <c r="C389" s="21"/>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A390" s="23" t="s">
+      <c r="A390" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B390" s="24"/>
-      <c r="C390" s="24"/>
+      <c r="B390" s="23"/>
+      <c r="C390" s="23"/>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A391" s="25" t="s">
+      <c r="A391" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B391" s="26"/>
-      <c r="C391" s="27"/>
+      <c r="B391" s="25"/>
+      <c r="C391" s="26"/>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
@@ -6908,11 +6908,11 @@
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A398" s="28" t="s">
+      <c r="A398" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B398" s="29"/>
-      <c r="C398" s="30"/>
+      <c r="B398" s="28"/>
+      <c r="C398" s="29"/>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
@@ -6992,11 +6992,11 @@
       </c>
     </row>
     <row r="408" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A408" s="22" t="s">
+      <c r="A408" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="B408" s="22"/>
-      <c r="C408" s="22"/>
+      <c r="B408" s="39"/>
+      <c r="C408" s="39"/>
     </row>
     <row r="409" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A409" s="8"/>
@@ -7286,83 +7286,18 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{808BDE38-2E40-4450-8137-228A8C80B0DE}" topLeftCell="A139">
+      <selection activeCell="A155" sqref="A155:C155"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{71292C98-6F74-4667-9CC4-FC968CFB3932}">
       <selection activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-    </customSheetView>
-    <customSheetView guid="{808BDE38-2E40-4450-8137-228A8C80B0DE}" topLeftCell="A139">
-      <selection activeCell="A155" sqref="A155:C155"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="81">
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A137:C137"/>
-    <mergeCell ref="A138:C138"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A102:C102"/>
-    <mergeCell ref="A109:C109"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="A146:C146"/>
-    <mergeCell ref="A174:C174"/>
-    <mergeCell ref="A175:C175"/>
-    <mergeCell ref="A176:C176"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A155:C155"/>
-    <mergeCell ref="A191:C191"/>
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A199:C199"/>
-    <mergeCell ref="A207:C207"/>
-    <mergeCell ref="A208:C208"/>
-    <mergeCell ref="A215:C215"/>
-    <mergeCell ref="A223:C223"/>
-    <mergeCell ref="A224:C224"/>
-    <mergeCell ref="A232:C232"/>
-    <mergeCell ref="A242:C242"/>
-    <mergeCell ref="A269:C269"/>
-    <mergeCell ref="A279:C279"/>
-    <mergeCell ref="A280:C280"/>
-    <mergeCell ref="A243:C243"/>
-    <mergeCell ref="A244:C244"/>
-    <mergeCell ref="A252:C252"/>
-    <mergeCell ref="A260:C260"/>
-    <mergeCell ref="A261:C261"/>
-    <mergeCell ref="A281:C281"/>
-    <mergeCell ref="A288:C288"/>
-    <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A297:C297"/>
-    <mergeCell ref="A304:C304"/>
-    <mergeCell ref="A389:C389"/>
-    <mergeCell ref="A390:C390"/>
-    <mergeCell ref="A391:C391"/>
-    <mergeCell ref="A312:C312"/>
-    <mergeCell ref="A313:C313"/>
-    <mergeCell ref="A321:C321"/>
-    <mergeCell ref="A370:C370"/>
-    <mergeCell ref="A371:C371"/>
     <mergeCell ref="A436:C436"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A419:C419"/>
@@ -7379,6 +7314,71 @@
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A372:C372"/>
     <mergeCell ref="A379:C379"/>
+    <mergeCell ref="A389:C389"/>
+    <mergeCell ref="A390:C390"/>
+    <mergeCell ref="A391:C391"/>
+    <mergeCell ref="A312:C312"/>
+    <mergeCell ref="A313:C313"/>
+    <mergeCell ref="A321:C321"/>
+    <mergeCell ref="A370:C370"/>
+    <mergeCell ref="A371:C371"/>
+    <mergeCell ref="A281:C281"/>
+    <mergeCell ref="A288:C288"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A297:C297"/>
+    <mergeCell ref="A304:C304"/>
+    <mergeCell ref="A269:C269"/>
+    <mergeCell ref="A279:C279"/>
+    <mergeCell ref="A280:C280"/>
+    <mergeCell ref="A243:C243"/>
+    <mergeCell ref="A244:C244"/>
+    <mergeCell ref="A252:C252"/>
+    <mergeCell ref="A260:C260"/>
+    <mergeCell ref="A261:C261"/>
+    <mergeCell ref="A215:C215"/>
+    <mergeCell ref="A223:C223"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A232:C232"/>
+    <mergeCell ref="A242:C242"/>
+    <mergeCell ref="A191:C191"/>
+    <mergeCell ref="A192:C192"/>
+    <mergeCell ref="A199:C199"/>
+    <mergeCell ref="A207:C207"/>
+    <mergeCell ref="A208:C208"/>
+    <mergeCell ref="A146:C146"/>
+    <mergeCell ref="A174:C174"/>
+    <mergeCell ref="A175:C175"/>
+    <mergeCell ref="A176:C176"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A155:C155"/>
+    <mergeCell ref="A137:C137"/>
+    <mergeCell ref="A138:C138"/>
+    <mergeCell ref="A139:C139"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A109:C109"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -7419,11 +7419,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{71292C98-6F74-4667-9CC4-FC968CFB3932}">
+    <customSheetView guid="{808BDE38-2E40-4450-8137-228A8C80B0DE}">
       <selection activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{808BDE38-2E40-4450-8137-228A8C80B0DE}">
+    <customSheetView guid="{71292C98-6F74-4667-9CC4-FC968CFB3932}">
       <selection activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>